<commit_message>
Add Map, Entities and Exceptions
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/Blueprints.xlsx
+++ b/Assets/StreamingAssets/Blueprints.xlsx
@@ -3,8 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="Animals" sheetId="1" r:id="rId5"/>
-    <sheet state="visible" name="DayNightCycle" sheetId="2" r:id="rId6"/>
+    <sheet state="visible" name="Tile Types" sheetId="1" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -12,72 +11,54 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="16">
   <si>
     <t>IDS</t>
   </si>
   <si>
-    <t>Life</t>
-  </si>
-  <si>
-    <t>Food</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Monkey</t>
-  </si>
-  <si>
-    <t>100,200</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>Pepe</t>
-  </si>
-  <si>
-    <t>Snake</t>
-  </si>
-  <si>
-    <t>25</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>Jose</t>
-  </si>
-  <si>
-    <t>Bird</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>Piolin</t>
-  </si>
-  <si>
-    <t>Duration</t>
-  </si>
-  <si>
-    <t>Manana</t>
-  </si>
-  <si>
-    <t>Mediodia</t>
-  </si>
-  <si>
-    <t>Atardecer</t>
-  </si>
-  <si>
-    <t>Anochecer</t>
-  </si>
-  <si>
-    <t>Madrugada</t>
+    <t>Is Structure</t>
+  </si>
+  <si>
+    <t>Is Walkable</t>
+  </si>
+  <si>
+    <t>Is Animal Habitat</t>
+  </si>
+  <si>
+    <t>Can Spawn Humans</t>
+  </si>
+  <si>
+    <t>Can Dispawn Humans</t>
+  </si>
+  <si>
+    <t>Is Default</t>
+  </si>
+  <si>
+    <t>Road</t>
+  </si>
+  <si>
+    <t>FALSE</t>
+  </si>
+  <si>
+    <t>TRUE</t>
+  </si>
+  <si>
+    <t>Jail wall</t>
+  </si>
+  <si>
+    <t>Jail habitat</t>
+  </si>
+  <si>
+    <t>Power Suply</t>
+  </si>
+  <si>
+    <t>Humans entry</t>
+  </si>
+  <si>
+    <t>Humans exit</t>
+  </si>
+  <si>
+    <t>Grass</t>
   </si>
 </sst>
 </file>
@@ -118,10 +99,10 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -131,10 +112,6 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -345,6 +322,11 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="4" max="4" width="14.75"/>
+    <col customWidth="1" min="5" max="5" width="17.25"/>
+    <col customWidth="1" min="6" max="6" width="21.0"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -359,144 +341,212 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="B6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="B7" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-    </row>
-    <row r="8">
-      <c r="B8" s="2"/>
-    </row>
-  </sheetData>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="3">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="3">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="3">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="3">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="3">
-        <v>4.0</v>
-      </c>
+      <c r="B8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
add a simple engine with GameObject, Components and Prefabs support
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/Blueprints.xlsx
+++ b/Assets/StreamingAssets/Blueprints.xlsx
@@ -4,6 +4,9 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="Tile Types" sheetId="1" r:id="rId5"/>
+    <sheet state="visible" name="DayNightCycle" sheetId="2" r:id="rId6"/>
+    <sheet state="visible" name="Animals" sheetId="3" r:id="rId7"/>
+    <sheet state="visible" name="PrefabsView" sheetId="4" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -11,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="29">
   <si>
     <t>IDS</t>
   </si>
@@ -59,6 +62,45 @@
   </si>
   <si>
     <t>Grass</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Duration</t>
+  </si>
+  <si>
+    <t>Morning</t>
+  </si>
+  <si>
+    <t>MidDay</t>
+  </si>
+  <si>
+    <t>Afternoon</t>
+  </si>
+  <si>
+    <t>Evening</t>
+  </si>
+  <si>
+    <t>Sunrise</t>
+  </si>
+  <si>
+    <t>Dusk</t>
+  </si>
+  <si>
+    <t>Monkey</t>
+  </si>
+  <si>
+    <t>Architecture ID</t>
+  </si>
+  <si>
+    <t>Prefab resource path</t>
+  </si>
+  <si>
+    <t>Monkey view</t>
+  </si>
+  <si>
+    <t>../Prefabs/Monkey.xml</t>
   </si>
 </sst>
 </file>
@@ -92,7 +134,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -103,6 +145,9 @@
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -112,6 +157,18 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -551,4 +608,473 @@
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="4">
+        <v>60.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="4">
+        <v>60.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="4">
+        <v>60.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="4">
+        <v>60.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="4">
+        <v>60.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="4">
+        <v>60.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="11.63"/>
+    <col customWidth="1" min="2" max="2" width="14.0"/>
+    <col customWidth="1" min="3" max="3" width="38.25"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Spawn entities from view
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/Blueprints.xlsx
+++ b/Assets/StreamingAssets/Blueprints.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="38">
   <si>
     <t>IDS</t>
   </si>
@@ -91,6 +91,15 @@
     <t>Monkey</t>
   </si>
   <si>
+    <t>Bird</t>
+  </si>
+  <si>
+    <t>Snake</t>
+  </si>
+  <si>
+    <t>Lion</t>
+  </si>
+  <si>
     <t>Architecture ID</t>
   </si>
   <si>
@@ -101,6 +110,24 @@
   </si>
   <si>
     <t>../Prefabs/Monkey.xml</t>
+  </si>
+  <si>
+    <t>Bird view</t>
+  </si>
+  <si>
+    <t>../Prefabs/Bird.xml</t>
+  </si>
+  <si>
+    <t>Snake view</t>
+  </si>
+  <si>
+    <t>../Prefabs/Snake.xml</t>
+  </si>
+  <si>
+    <t>Lion view</t>
+  </si>
+  <si>
+    <t>../Prefabs/Lion.xml</t>
   </si>
 </sst>
 </file>
@@ -747,8 +774,12 @@
       <c r="K2" s="3"/>
     </row>
     <row r="3">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
+      <c r="A3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
@@ -760,8 +791,12 @@
       <c r="K3" s="3"/>
     </row>
     <row r="4">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
+      <c r="A4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
@@ -773,8 +808,12 @@
       <c r="K4" s="3"/>
     </row>
     <row r="5">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
+      <c r="A5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
@@ -1057,21 +1096,54 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>24</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>28</v>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Scene GameScene MapView Grid and refactor GameObjects
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/Blueprints.xlsx
+++ b/Assets/StreamingAssets/Blueprints.xlsx
@@ -4,9 +4,10 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="Tile Types" sheetId="1" r:id="rId5"/>
-    <sheet state="visible" name="DayNightCycle" sheetId="2" r:id="rId6"/>
-    <sheet state="visible" name="Animals" sheetId="3" r:id="rId7"/>
-    <sheet state="visible" name="PrefabsView" sheetId="4" r:id="rId8"/>
+    <sheet state="visible" name="Tiles View" sheetId="2" r:id="rId6"/>
+    <sheet state="visible" name="DayNightCycle" sheetId="3" r:id="rId7"/>
+    <sheet state="visible" name="Animals" sheetId="4" r:id="rId8"/>
+    <sheet state="visible" name="Prefabs View" sheetId="5" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -14,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="51">
   <si>
     <t>IDS</t>
   </si>
@@ -64,6 +65,51 @@
     <t>Grass</t>
   </si>
   <si>
+    <t>Architecture ID</t>
+  </si>
+  <si>
+    <t>Prefab resource path</t>
+  </si>
+  <si>
+    <t>Road View</t>
+  </si>
+  <si>
+    <t>../Prefabs/Map/YellowTile.xml</t>
+  </si>
+  <si>
+    <t>Jail walls View</t>
+  </si>
+  <si>
+    <t>Jail walls</t>
+  </si>
+  <si>
+    <t>../Prefabs/Map/RedTile.xml</t>
+  </si>
+  <si>
+    <t>Jail habitat View</t>
+  </si>
+  <si>
+    <t>../Prefabs/Map/LightblueTile.xml</t>
+  </si>
+  <si>
+    <t>Power Suply View</t>
+  </si>
+  <si>
+    <t>../Prefabs/Map/WhiteTile.xml</t>
+  </si>
+  <si>
+    <t>Humans entry View</t>
+  </si>
+  <si>
+    <t>Humans exit View</t>
+  </si>
+  <si>
+    <t>Grass View</t>
+  </si>
+  <si>
+    <t>../Prefabs/Map/GreenTile.xml</t>
+  </si>
+  <si>
     <t>Name</t>
   </si>
   <si>
@@ -98,12 +144,6 @@
   </si>
   <si>
     <t>Lion</t>
-  </si>
-  <si>
-    <t>Architecture ID</t>
-  </si>
-  <si>
-    <t>Prefab resource path</t>
   </si>
   <si>
     <t>Monkey view</t>
@@ -134,7 +174,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -145,6 +185,10 @@
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -161,7 +205,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -175,6 +219,12 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -196,6 +246,10 @@
 </file>
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -646,6 +700,9 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="3" max="3" width="30.75"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="4" t="s">
@@ -659,69 +716,80 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="4">
-        <v>60.0</v>
+      <c r="B2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="4">
-        <v>60.0</v>
+      <c r="A3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="4">
-        <v>60.0</v>
+      <c r="A4" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="4">
-        <v>60.0</v>
+      <c r="A5" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="4">
-        <v>60.0</v>
+      <c r="A6" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="4">
-        <v>60.0</v>
+      <c r="A7" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -730,6 +798,98 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="4">
+        <v>60.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="4">
+        <v>60.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="4">
+        <v>60.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="4">
+        <v>60.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="4">
+        <v>60.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="4">
+        <v>60.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -744,7 +904,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -758,10 +918,10 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -775,10 +935,10 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -792,10 +952,10 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -809,10 +969,10 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -1076,7 +1236,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -1096,54 +1256,54 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>